<commit_message>
Well Dynamic TF on Qt
</commit_message>
<xml_diff>
--- a/ABB.xlsx
+++ b/ABB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\AllThingsPython\1.DD_GLO\modbus-sim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\AllThingsPython\modbus-net\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F856C5-3670-48B2-ADC0-DB8C29545B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BFB94D-451A-4964-A537-C4B7D00BD7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FF54B6BA-5851-451C-92B8-85953EE59363}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="105">
   <si>
     <t>Description</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>GLIR B</t>
+  </si>
+  <si>
+    <t>GLIR A</t>
   </si>
 </sst>
 </file>
@@ -909,7 +912,7 @@
   <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1118,7 @@
         <v>4321</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="H5" s="11">
         <v>2</v>
@@ -1414,7 +1417,7 @@
         <v>52</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>38</v>

</xml_diff>